<commit_message>
removed first column not needed
</commit_message>
<xml_diff>
--- a/doc/Crosswalk of registries information models.xlsx
+++ b/doc/Crosswalk of registries information models.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miriam.baglioni/Develop/Gitea/RegistriesOverlap/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miriam.baglioni/Develop/gitHub/scholarly_repository_registry_interoperability/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7288A24-CB77-5E4A-B6AA-6DA587B09DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A404A6-D944-1E48-B219-5A6D7EE2A6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="4700" windowWidth="32220" windowHeight="18000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2140" yWindow="4700" windowWidth="32220" windowHeight="18000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="154">
   <si>
     <t>Macro-area</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Generality</t>
   </si>
   <si>
     <t xml:space="preserve">This macro area groups all the generic information that identifies and describes individual records (in the case of this analysis: repositories) within a registry. Such as: id (or similar), name, description, url </t>
@@ -278,9 +275,6 @@
   </si>
   <si>
     <t>Definition</t>
-  </si>
-  <si>
-    <t>Content classification</t>
   </si>
   <si>
     <t xml:space="preserve"> All the information describing the area, discipline or scientific domain of reference, including tags and labels.</t>
@@ -309,15 +303,9 @@
 focus of repository.</t>
   </si>
   <si>
-    <t>Macro area</t>
-  </si>
-  <si>
     <t>Fairsharing</t>
   </si>
   <si>
-    <t>Technical info</t>
-  </si>
-  <si>
     <t>API, versioning and other fields for machine/programmatic interoperability</t>
   </si>
   <si>
@@ -363,9 +351,6 @@
     <t>Mapping when compatible types are specified</t>
   </si>
   <si>
-    <t>Dates and times</t>
-  </si>
-  <si>
     <t>Information describing the uptodateness of the repository</t>
   </si>
   <si>
@@ -394,9 +379,6 @@
   </si>
   <si>
     <t>The date of the last update of the repository</t>
-  </si>
-  <si>
-    <t>Legal aspects</t>
   </si>
   <si>
     <t>This macro area contains information on the type of access (ie. open, closed, restricted), licences or policies adopted by the single record.</t>
@@ -589,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -641,6 +623,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -860,60 +845,56 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" customWidth="1"/>
-    <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="39.83203125" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="31.1640625" customWidth="1"/>
-    <col min="7" max="7" width="59.83203125" customWidth="1"/>
+    <col min="1" max="1" width="39" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="39.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" customWidth="1"/>
+    <col min="6" max="6" width="59.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="17" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="17"/>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="17"/>
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -927,14 +908,14 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="17"/>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="17"/>
       <c r="C4" t="s">
         <v>15</v>
       </c>
@@ -948,47 +929,47 @@
         <v>18</v>
       </c>
       <c r="G4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="17"/>
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="17"/>
       <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>21</v>
       </c>
       <c r="G5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="17"/>
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="H5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="17"/>
       <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>24</v>
       </c>
       <c r="F6" t="s">
         <v>25</v>
       </c>
       <c r="G6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="17"/>
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="17"/>
       <c r="C7" t="s">
         <v>27</v>
       </c>
@@ -1004,35 +985,35 @@
       <c r="G7" t="s">
         <v>31</v>
       </c>
-      <c r="H7" t="s">
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="17"/>
+      <c r="B8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="17"/>
       <c r="C8" t="s">
         <v>33</v>
       </c>
       <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
         <v>34</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
       </c>
       <c r="G8" t="s">
         <v>35</v>
       </c>
-      <c r="H8" t="s">
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="17"/>
+      <c r="B9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="17"/>
-      <c r="C9" t="s">
-        <v>37</v>
+      <c r="D9" t="s">
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
         <v>37</v>
@@ -1040,56 +1021,53 @@
       <c r="G9" t="s">
         <v>38</v>
       </c>
-      <c r="H9" t="s">
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="17"/>
+      <c r="C10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="17"/>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>40</v>
       </c>
       <c r="F10" t="s">
         <v>41</v>
       </c>
       <c r="G10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="H10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C11" t="s">
         <v>43</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>44</v>
       </c>
       <c r="G11" t="s">
         <v>45</v>
       </c>
-      <c r="H11" t="s">
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D12" t="s">
         <v>47</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>48</v>
       </c>
       <c r="G12" t="s">
         <v>49</v>
       </c>
-      <c r="H12" t="s">
-        <v>50</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="A2:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1100,93 +1078,91 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>94</v>
+        <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="20"/>
+      <c r="B3" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="8"/>
-      <c r="C3" s="15" t="s">
+      <c r="G3" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="20"/>
+      <c r="B4" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="C4" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="D4" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F4" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C4" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1241,149 +1217,149 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>52</v>
-      </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="18"/>
       <c r="C3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="18"/>
       <c r="C4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>60</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="12"/>
       <c r="G4" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="18"/>
       <c r="C5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="E5" s="8"/>
       <c r="G5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="18"/>
       <c r="C6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="18"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="18"/>
       <c r="C8" s="7"/>
       <c r="D8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="18"/>
       <c r="C9" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1413,97 +1389,90 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B4"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="2" width="32.1640625" customWidth="1"/>
-    <col min="6" max="6" width="22.1640625" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="19"/>
+      <c r="B3" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="C3" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="19"/>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="19"/>
+      <c r="B4" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="E4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="19"/>
-      <c r="C4" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A2:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1514,124 +1483,118 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="29.1640625" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="17"/>
+      <c r="B3" t="s">
         <v>93</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="C3" t="s">
         <v>94</v>
       </c>
-      <c r="G1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+      <c r="D3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="G3" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="17"/>
+      <c r="B4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="17"/>
-      <c r="C3" t="s">
+      <c r="E4" t="s">
         <v>97</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F4" t="s">
         <v>98</v>
       </c>
-      <c r="E3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>99</v>
       </c>
-      <c r="H3" s="16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="17"/>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="17"/>
+      <c r="B5" t="s">
         <v>100</v>
       </c>
-      <c r="F4" t="s">
+      <c r="C5" t="s">
         <v>101</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F5" t="s">
         <v>102</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="17"/>
+      <c r="B6" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="17"/>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>104</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>105</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F6" t="s">
         <v>106</v>
       </c>
-      <c r="H5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="17"/>
-      <c r="C6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E6" t="s">
-        <v>109</v>
-      </c>
       <c r="G6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A2:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1642,171 +1605,165 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="36.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" customWidth="1"/>
-    <col min="12" max="12" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="36.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="F1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="G1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="17"/>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="17"/>
+      <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="E4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="17"/>
-      <c r="C3" t="s">
+      <c r="F4" t="s">
         <v>124</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G4" s="16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="17"/>
+      <c r="B5" t="s">
         <v>125</v>
       </c>
-      <c r="G3" t="s">
+      <c r="E5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" t="s">
         <v>126</v>
       </c>
-      <c r="H3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="17"/>
-      <c r="C4" t="s">
+      <c r="G5" t="s">
         <v>127</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="17"/>
+      <c r="B6" t="s">
         <v>128</v>
       </c>
-      <c r="F4" t="s">
+      <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" t="s">
         <v>129</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F6" t="s">
         <v>130</v>
       </c>
-      <c r="H4" s="16" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="17"/>
-      <c r="C5" t="s">
+      <c r="G6" t="s">
         <v>131</v>
       </c>
-      <c r="F5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="17"/>
+      <c r="B7" t="s">
         <v>132</v>
       </c>
-      <c r="H5" t="s">
+      <c r="E7" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="17"/>
-      <c r="C6" t="s">
+      <c r="F7" t="s">
         <v>134</v>
       </c>
-      <c r="D6" t="s">
-        <v>128</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="G7" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="17"/>
+      <c r="B8" t="s">
         <v>135</v>
       </c>
-      <c r="G6" t="s">
+      <c r="E8" t="s">
         <v>136</v>
       </c>
-      <c r="H6" t="s">
+      <c r="F8" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="17"/>
-      <c r="C7" t="s">
+      <c r="G8" s="16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="17"/>
+      <c r="B9" t="s">
         <v>138</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E9" t="s">
         <v>139</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F9" t="s">
         <v>140</v>
       </c>
-      <c r="H7" s="16" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="17"/>
-      <c r="C8" t="s">
+      <c r="G9" t="s">
         <v>141</v>
-      </c>
-      <c r="F8" t="s">
-        <v>142</v>
-      </c>
-      <c r="G8" t="s">
-        <v>143</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="17"/>
-      <c r="C9" t="s">
-        <v>144</v>
-      </c>
-      <c r="F9" t="s">
-        <v>145</v>
-      </c>
-      <c r="G9" t="s">
-        <v>146</v>
-      </c>
-      <c r="H9" t="s">
-        <v>147</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="A2:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>